<commit_message>
Add in ability for full economy (multiple industry sectors) to be processed in one go.
- Added priority to batch recipe to determine order of execution for industry sectors.
- Added library classes for industries, recipes and trade goods. Allows internal handling via name rather than via guid.
</commit_message>
<xml_diff>
--- a/doc/Trade Goods.xlsx
+++ b/doc/Trade Goods.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Trade goods" sheetId="1" r:id="rId1"/>
@@ -905,10 +905,6 @@
     <t>Standard 1.0 = roughly 240kg per person per annum = 20kg per cycle.</t>
   </si>
   <si>
-    <t>Standard 1.0 = roughly 1080kg per person per annum = 90kg per cycle.
-Assumes recycling of things such as air and water is around 99.9%</t>
-  </si>
-  <si>
     <t>Standard 1.0 = roughly 120kg per person per annum = 10kg per cycle.</t>
   </si>
   <si>
@@ -1028,6 +1024,10 @@
   <si>
     <t>Precursor ruins automatically generate this trade good "for free / no workers" depending on ruin size.
 This should also not be "consumed" but rather build up over time. So treat like a service that requires this trade good to construct, rather than consuming it directly.</t>
+  </si>
+  <si>
+    <t>Standard 1.0 = roughly 1080kg per person per annum = 90kg per cycle.
+So assuming that recycling of things such as air and water is around 99.9% = 0.09kg</t>
   </si>
 </sst>
 </file>
@@ -1295,36 +1295,6 @@
     <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="82">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1805,6 +1775,36 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -8022,122 +8022,122 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table2567" displayName="Table2567" ref="B10:X31" totalsRowShown="0" dataDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table2567" displayName="Table2567" ref="B10:X31" totalsRowShown="0" dataDxfId="67">
   <autoFilter ref="B10:X31"/>
   <sortState ref="B5:I21">
     <sortCondition ref="E24:E41"/>
   </sortState>
   <tableColumns count="23">
-    <tableColumn id="1" name="Industry / Service" dataDxfId="72"/>
-    <tableColumn id="3" name="Type" dataDxfId="71"/>
-    <tableColumn id="8" name="IndL" dataDxfId="70"/>
-    <tableColumn id="5" name="Minimum industry level" dataDxfId="69"/>
-    <tableColumn id="4" name="Requirements" dataDxfId="68"/>
-    <tableColumn id="7" name="Notes" dataDxfId="67"/>
-    <tableColumn id="2" name="Good 1" dataDxfId="66">
+    <tableColumn id="1" name="Industry / Service" dataDxfId="66"/>
+    <tableColumn id="3" name="Type" dataDxfId="65"/>
+    <tableColumn id="8" name="IndL" dataDxfId="64"/>
+    <tableColumn id="5" name="Minimum industry level" dataDxfId="63"/>
+    <tableColumn id="4" name="Requirements" dataDxfId="62"/>
+    <tableColumn id="7" name="Notes" dataDxfId="61"/>
+    <tableColumn id="2" name="Good 1" dataDxfId="60">
       <calculatedColumnFormula>'Trade goods'!H11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Val 1" dataDxfId="65">
+    <tableColumn id="6" name="Val 1" dataDxfId="59">
       <calculatedColumnFormula>Consumption!C7 * 1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Good 2" dataDxfId="64">
+    <tableColumn id="9" name="Good 2" dataDxfId="58">
       <calculatedColumnFormula>'Trade goods'!H12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Val 2" dataDxfId="63"/>
-    <tableColumn id="11" name="Good 3" dataDxfId="62">
+    <tableColumn id="10" name="Val 2" dataDxfId="57"/>
+    <tableColumn id="11" name="Good 3" dataDxfId="56">
       <calculatedColumnFormula>'Trade goods'!H12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Val 3" dataDxfId="61"/>
-    <tableColumn id="13" name="Good 4" dataDxfId="60">
+    <tableColumn id="12" name="Val 3" dataDxfId="55"/>
+    <tableColumn id="13" name="Good 4" dataDxfId="54">
       <calculatedColumnFormula>'Trade goods'!H8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Val 4" dataDxfId="59"/>
-    <tableColumn id="15" name="Good 5" dataDxfId="58"/>
-    <tableColumn id="16" name="Val 5" dataDxfId="57"/>
-    <tableColumn id="18" name="Labour (PiM per set)" dataDxfId="56"/>
-    <tableColumn id="19" name="Set Size" dataDxfId="55"/>
-    <tableColumn id="23" name="Cost per Set (Work)" dataDxfId="54"/>
-    <tableColumn id="24" name="Cost per Set (Materials)" dataDxfId="53"/>
-    <tableColumn id="20" name="Cost per Set (Other)" dataDxfId="52"/>
-    <tableColumn id="21" name="Maximum count" dataDxfId="51"/>
-    <tableColumn id="17" name="Civilian Expansion Rules" dataDxfId="50"/>
+    <tableColumn id="14" name="Val 4" dataDxfId="53"/>
+    <tableColumn id="15" name="Good 5" dataDxfId="52"/>
+    <tableColumn id="16" name="Val 5" dataDxfId="51"/>
+    <tableColumn id="18" name="Labour (PiM per set)" dataDxfId="50"/>
+    <tableColumn id="19" name="Set Size" dataDxfId="49"/>
+    <tableColumn id="23" name="Cost per Set (Work)" dataDxfId="48"/>
+    <tableColumn id="24" name="Cost per Set (Materials)" dataDxfId="47"/>
+    <tableColumn id="20" name="Cost per Set (Other)" dataDxfId="46"/>
+    <tableColumn id="21" name="Maximum count" dataDxfId="45"/>
+    <tableColumn id="17" name="Civilian Expansion Rules" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table39" displayName="Table39" ref="B4:F15" totalsRowShown="0" headerRowDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table39" displayName="Table39" ref="B4:F15" totalsRowShown="0" headerRowDxfId="43">
   <autoFilter ref="B4:F15"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="48"/>
-    <tableColumn id="5" name="Level" dataDxfId="47"/>
-    <tableColumn id="2" name="Min Value" dataDxfId="46"/>
-    <tableColumn id="3" name="Effects" dataDxfId="45"/>
-    <tableColumn id="4" name="Description" dataDxfId="44"/>
+    <tableColumn id="1" name="#" dataDxfId="42"/>
+    <tableColumn id="5" name="Level" dataDxfId="41"/>
+    <tableColumn id="2" name="Min Value" dataDxfId="40"/>
+    <tableColumn id="3" name="Effects" dataDxfId="39"/>
+    <tableColumn id="4" name="Description" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B4:I15" totalsRowShown="0" headerRowDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B4:I15" totalsRowShown="0" headerRowDxfId="37">
   <autoFilter ref="B4:I15"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Level" dataDxfId="42"/>
-    <tableColumn id="2" name="Min Value" dataDxfId="41"/>
-    <tableColumn id="5" name="PiM Tax Modifier" dataDxfId="40"/>
-    <tableColumn id="6" name="Research Modifier" dataDxfId="39"/>
-    <tableColumn id="3" name="Effects" dataDxfId="38"/>
-    <tableColumn id="8" name="Description" dataDxfId="37"/>
-    <tableColumn id="4" name="Population growth modifier" dataDxfId="36"/>
-    <tableColumn id="9" name="Population die-off modifier" dataDxfId="35"/>
+    <tableColumn id="1" name="Level" dataDxfId="36"/>
+    <tableColumn id="2" name="Min Value" dataDxfId="35"/>
+    <tableColumn id="5" name="PiM Tax Modifier" dataDxfId="34"/>
+    <tableColumn id="6" name="Research Modifier" dataDxfId="33"/>
+    <tableColumn id="3" name="Effects" dataDxfId="32"/>
+    <tableColumn id="8" name="Description" dataDxfId="31"/>
+    <tableColumn id="4" name="Population growth modifier" dataDxfId="30"/>
+    <tableColumn id="9" name="Population die-off modifier" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table38" displayName="Table38" ref="B6:O30" totalsRowShown="0" headerRowDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table38" displayName="Table38" ref="B6:O30" totalsRowShown="0" headerRowDxfId="28">
   <autoFilter ref="B6:O30"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="Trade Good / Service" dataDxfId="33">
+    <tableColumn id="1" name="Trade Good / Service" dataDxfId="27">
       <calculatedColumnFormula>'Trade goods'!B11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Base Consumption per PiM per Cycle" dataDxfId="32"/>
-    <tableColumn id="3" name="Death-spiral" dataDxfId="31"/>
-    <tableColumn id="4" name="Abysmal" dataDxfId="30"/>
-    <tableColumn id="5" name="Poverty stricken" dataDxfId="29"/>
-    <tableColumn id="6" name="Subsistence" dataDxfId="28"/>
-    <tableColumn id="7" name="Standard" dataDxfId="27"/>
-    <tableColumn id="8" name="Abundant" dataDxfId="26"/>
-    <tableColumn id="9" name="Luxurious" dataDxfId="25"/>
-    <tableColumn id="10" name="Post-Scarcity" dataDxfId="24"/>
-    <tableColumn id="11" name="Post-Luxury" dataDxfId="23"/>
-    <tableColumn id="12" name="Decadent" dataDxfId="22"/>
-    <tableColumn id="13" name="Post-Decadent" dataDxfId="21"/>
-    <tableColumn id="14" name="Note" dataDxfId="20"/>
+    <tableColumn id="2" name="Base Consumption per PiM per Cycle" dataDxfId="26"/>
+    <tableColumn id="3" name="Death-spiral" dataDxfId="25"/>
+    <tableColumn id="4" name="Abysmal" dataDxfId="24"/>
+    <tableColumn id="5" name="Poverty stricken" dataDxfId="23"/>
+    <tableColumn id="6" name="Subsistence" dataDxfId="22"/>
+    <tableColumn id="7" name="Standard" dataDxfId="21"/>
+    <tableColumn id="8" name="Abundant" dataDxfId="20"/>
+    <tableColumn id="9" name="Luxurious" dataDxfId="19"/>
+    <tableColumn id="10" name="Post-Scarcity" dataDxfId="18"/>
+    <tableColumn id="11" name="Post-Luxury" dataDxfId="17"/>
+    <tableColumn id="12" name="Decadent" dataDxfId="16"/>
+    <tableColumn id="13" name="Post-Decadent" dataDxfId="15"/>
+    <tableColumn id="14" name="Note" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B5:K8" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B5:K8" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10">
   <autoFilter ref="B5:K8"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="Megaproject" dataDxfId="15"/>
-    <tableColumn id="2" name="Automatically trades SN-goods between all planets in the system._x000a_Requires High Tech to build._x000a_Very low upkeep cost of High Tech." dataDxfId="14"/>
-    <tableColumn id="3" name="IndL" dataDxfId="13"/>
-    <tableColumn id="4" name="Minimum industry level" dataDxfId="12">
+    <tableColumn id="1" name="Megaproject" dataDxfId="9"/>
+    <tableColumn id="2" name="Automatically trades SN-goods between all planets in the system._x000a_Requires High Tech to build._x000a_Very low upkeep cost of High Tech." dataDxfId="8"/>
+    <tableColumn id="3" name="IndL" dataDxfId="7"/>
+    <tableColumn id="4" name="Minimum industry level" dataDxfId="6">
       <calculatedColumnFormula>VLOOKUP(D6,Table39[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Labour (PiM)" dataDxfId="11"/>
-    <tableColumn id="7" name="Cost (Work)" dataDxfId="10"/>
-    <tableColumn id="8" name="Cost (Materials)" dataDxfId="9"/>
-    <tableColumn id="9" name="Cost (Other)" dataDxfId="8"/>
-    <tableColumn id="10" name="Upkeep (per annum)" dataDxfId="7"/>
-    <tableColumn id="11" name="Additional Information" dataDxfId="6"/>
+    <tableColumn id="5" name="Labour (PiM)" dataDxfId="5"/>
+    <tableColumn id="7" name="Cost (Work)" dataDxfId="4"/>
+    <tableColumn id="8" name="Cost (Materials)" dataDxfId="3"/>
+    <tableColumn id="9" name="Cost (Other)" dataDxfId="2"/>
+    <tableColumn id="10" name="Upkeep (per annum)" dataDxfId="1"/>
+    <tableColumn id="11" name="Additional Information" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8424,8 +8424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8520,7 +8520,7 @@
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>194</v>
@@ -8675,7 +8675,7 @@
         <v>Full Industry</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>225</v>
@@ -8792,8 +8792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X43"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9081,7 +9081,7 @@
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H12" s="1" t="str">
         <f>'Trade goods'!H12</f>
@@ -9142,8 +9142,8 @@
         <v>209</v>
       </c>
       <c r="H13" s="1" t="str">
-        <f>Table25[[#This Row],[Internal Name]]</f>
-        <v>TG_NELR</v>
+        <f>'Trade goods'!H12</f>
+        <v>TG_NELC</v>
       </c>
       <c r="I13" s="23">
         <v>0.98</v>
@@ -9217,8 +9217,8 @@
         <v>-4.9000000000000004</v>
       </c>
       <c r="L14" s="1" t="str">
-        <f>Table25[[#This Row],[Internal Name]]</f>
-        <v>TG_WAST</v>
+        <f>'Trade goods'!H13</f>
+        <v>TG_NELR</v>
       </c>
       <c r="M14" s="23">
         <v>-0.1</v>
@@ -10183,32 +10183,32 @@
     <mergeCell ref="C40:O40"/>
   </mergeCells>
   <conditionalFormatting sqref="I11:I31">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="73" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:K31">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="72" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11:M15 M17:M31">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="71" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11:O31">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="70" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q11:Q31">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="69" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M16">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="68" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10475,10 +10475,10 @@
         <v>107</v>
       </c>
       <c r="D4" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>310</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>311</v>
       </c>
       <c r="F4" s="15" t="s">
         <v>158</v>
@@ -10487,10 +10487,10 @@
         <v>118</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="2:14" ht="30" x14ac:dyDescent="0.25">
@@ -10507,7 +10507,7 @@
         <v>-10000</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="40">
@@ -10531,7 +10531,7 @@
         <v>-100</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="40">
@@ -10543,7 +10543,7 @@
     </row>
     <row r="7" spans="2:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C7" s="14">
         <v>200</v>
@@ -10556,7 +10556,7 @@
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H7" s="40">
         <v>50</v>
@@ -10674,7 +10674,7 @@
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H12" s="40">
         <v>-150</v>
@@ -10698,7 +10698,7 @@
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H13" s="40">
         <v>-200</v>
@@ -10753,38 +10753,38 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="49" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C17" s="49"/>
       <c r="D17" s="41">
         <v>0.05</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="49" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C18" s="49"/>
       <c r="D18" s="41">
         <v>0.03</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D19" s="41">
         <f>D17-D18</f>
         <v>2.0000000000000004E-2</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -10797,18 +10797,18 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
@@ -10823,12 +10823,12 @@
     </row>
     <row r="29" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -10943,7 +10943,7 @@
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C63" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
@@ -10963,7 +10963,7 @@
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C68" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
@@ -10994,8 +10994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11096,7 +11096,7 @@
         <v>109</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G6" s="18" t="s">
         <v>110</v>
@@ -11178,7 +11178,7 @@
         <v>4</v>
       </c>
       <c r="O7" s="15" t="s">
-        <v>290</v>
+        <v>329</v>
       </c>
       <c r="Q7">
         <f>Table38[[#This Row],[Base Consumption per PiM per Cycle]] * 12 * $N$3 / 1000000 * 1000</f>
@@ -11294,7 +11294,7 @@
         <v>10</v>
       </c>
       <c r="O9" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Q9">
         <f>Table38[[#This Row],[Base Consumption per PiM per Cycle]] * 12 * $N$3 / 1000000 * 1000</f>
@@ -12768,38 +12768,38 @@
   <sheetData>
     <row r="2" spans="2:21" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="42" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K2" s="42" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="U2" s="42" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B38" s="50" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C38" s="50"/>
       <c r="D38" s="44" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="B39" s="42" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I39" s="42" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P39" s="42" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B40" s="43">
         <v>100</v>
@@ -12823,37 +12823,37 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B41" s="43" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C41" s="43">
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E41">
         <v>1</v>
       </c>
       <c r="I41" s="43" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J41" s="43">
         <v>2</v>
       </c>
       <c r="K41" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L41">
         <v>1</v>
       </c>
       <c r="P41" s="43" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q41" s="43">
         <v>2</v>
       </c>
       <c r="R41" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="S41">
         <v>1</v>
@@ -12861,37 +12861,37 @@
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B42" s="43" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C42" s="43">
         <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="I42" s="43" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J42" s="43">
         <v>20</v>
       </c>
       <c r="K42" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L42">
         <v>0</v>
       </c>
       <c r="P42" s="43" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q42" s="43">
         <v>50</v>
       </c>
       <c r="R42" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="S42">
         <v>0</v>
@@ -12899,37 +12899,37 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B43" s="43" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C43" s="43">
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E43">
         <v>1000</v>
       </c>
       <c r="I43" s="43" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J43" s="43">
         <v>1</v>
       </c>
       <c r="K43" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L43">
         <v>1000</v>
       </c>
       <c r="P43" s="43" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q43" s="43">
         <v>1</v>
       </c>
       <c r="R43" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="S43">
         <v>1000</v>
@@ -12937,31 +12937,31 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C44" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D44" t="s">
+        <v>314</v>
+      </c>
+      <c r="I44" t="s">
         <v>315</v>
       </c>
-      <c r="I44" t="s">
-        <v>316</v>
-      </c>
       <c r="J44" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K44" t="s">
+        <v>314</v>
+      </c>
+      <c r="P44" t="s">
         <v>315</v>
       </c>
-      <c r="P44" t="s">
-        <v>316</v>
-      </c>
       <c r="Q44" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="R44" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>